<commit_message>
update dufflebag unzipping max goal figure format
</commit_message>
<xml_diff>
--- a/real_robot_data_plots_and_demos/comparison_experiments/comparison_data_summary_spreadsheet_w_charts.xlsx
+++ b/real_robot_data_plots_and_demos/comparison_experiments/comparison_data_summary_spreadsheet_w_charts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janak\Documents\GitHub\closed_chain_affordance\real_robot_data_plots_and_demos\comparison_experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31593C41-4BC0-4210-90E9-6FC85D031E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC9822E8-CBE3-4297-854C-794F5EF8B50E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,12 +52,13 @@
     <definedName name="_xlchart.v1.39" hidden="1">data_summary!$E$1:$E$2</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">data_summary!$H$8:$H$12</definedName>
     <definedName name="_xlchart.v1.40" hidden="1">data_summary!$F$1:$F$2</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">(data_summary!$D$4,data_summary!$D$9:$D$10,data_summary!$D$12,data_summary!$D$15:$D$17)</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">(data_summary!$E$4,data_summary!$E$9:$E$10,data_summary!$E$12,data_summary!$E$15:$E$17)</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">(data_summary!$F$4,data_summary!$F$9:$F$10,data_summary!$F$12,data_summary!$F$15:$F$17)</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">data_summary!$D$1:$D$2</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">data_summary!$E$1:$E$2</definedName>
-    <definedName name="_xlchart.v1.46" hidden="1">data_summary!$F$1:$F$2</definedName>
+    <definedName name="_xlchart.v1.41" hidden="1">data_summary!$G$1:$G$2</definedName>
+    <definedName name="_xlchart.v1.42" hidden="1">data_summary!$G$2</definedName>
+    <definedName name="_xlchart.v1.43" hidden="1">data_summary!$G$8:$G$12</definedName>
+    <definedName name="_xlchart.v1.44" hidden="1">data_summary!$H$1:$H$2</definedName>
+    <definedName name="_xlchart.v1.45" hidden="1">data_summary!$H$8:$H$12</definedName>
+    <definedName name="_xlchart.v1.46" hidden="1">data_summary!$I$1:$I$2</definedName>
+    <definedName name="_xlchart.v1.47" hidden="1">data_summary!$I$8:$I$12</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">data_summary!$I$1:$I$2</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">data_summary!$I$8:$I$12</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">data_summary!$G$1:$G$2</definedName>
@@ -879,34 +880,51 @@
   <cx:chart>
     <cx:title pos="t" align="ctr" overlay="0">
       <cx:tx>
-        <cx:txData>
-          <cx:v>Dufflebag Unzipping Experiment Max Achievable Task Goals</cx:v>
-        </cx:txData>
+        <cx:rich>
+          <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr sz="1400" b="1" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Dufflebag Unzipping Experiment Max Achievable Task </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr sz="1400" b="1" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Goals</a:t>
+            </a:r>
+          </a:p>
+        </cx:rich>
       </cx:tx>
-      <cx:txPr>
-        <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr" rtl="0">
-            <a:defRPr sz="1400" b="1" i="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="1">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Dufflebag Unzipping Experiment Max Achievable Task Goals</a:t>
-          </a:r>
-        </a:p>
-      </cx:txPr>
     </cx:title>
     <cx:plotArea>
       <cx:plotAreaRegion>
@@ -929,6 +947,8 @@
             </a:ln>
           </cx:spPr>
           <cx:dataLabels>
+            <cx:visibility seriesName="0" categoryName="0" value="0"/>
+            <cx:separator>, </cx:separator>
             <cx:dataLabel idx="0">
               <cx:visibility seriesName="0" categoryName="0" value="0"/>
               <cx:separator>, </cx:separator>
@@ -961,18 +981,15 @@
                       </a:solidFill>
                     </a:defRPr>
                   </a:pPr>
-                  <a:r>
-                    <a:rPr lang="en-US" sz="900" b="1" i="0" u="none" strike="noStrike" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1"/>
-                      </a:solidFill>
-                      <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-                    </a:rPr>
-                    <a:t>0.25</a:t>
-                  </a:r>
+                  <a:endParaRPr lang="en-US" sz="900" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                  </a:endParaRPr>
                 </a:p>
               </cx:txPr>
-              <cx:visibility seriesName="0" categoryName="0" value="1"/>
+              <cx:visibility seriesName="0" categoryName="0" value="0"/>
               <cx:separator>, </cx:separator>
             </cx:dataLabel>
           </cx:dataLabels>
@@ -6654,6 +6671,76 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>448181</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>74346</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>199882</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>116321</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="TextBox 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8784D760-A7F3-4145-8039-45F3D8B8BFC8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8283529" y="9218346"/>
+          <a:ext cx="704201" cy="232475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="900" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>0.25</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6956,8 +7043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26412DA8-AF8B-424F-9A42-3270986B77E9}">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="R59" sqref="R59"/>
+    <sheetView tabSelected="1" topLeftCell="B28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N59" sqref="N59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>